<commit_message>
updating to new dataset
</commit_message>
<xml_diff>
--- a/notebooks/2020_data.xlsx
+++ b/notebooks/2020_data.xlsx
@@ -1,27 +1,21 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="23328"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4505"/>
   <workbookPr defaultThemeVersion="124226"/>
-  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-    <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Data_science\colaberry\MIT_Solve_dashboard\notebooks\"/>
-    </mc:Choice>
-  </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{836D4C84-05BB-4C71-A34B-02620B91ABCC}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-98" yWindow="-98" windowWidth="20715" windowHeight="13276" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="240" yWindow="15" windowWidth="16095" windowHeight="9660"/>
   </bookViews>
   <sheets>
     <sheet name="Partner Data" sheetId="1" r:id="rId1"/>
     <sheet name="Solver Team Data" sheetId="2" r:id="rId2"/>
   </sheets>
-  <calcPr calcId="124519"/>
+  <calcPr calcId="124519" fullCalcOnLoad="1"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="963" uniqueCount="262">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1227" uniqueCount="272">
   <si>
     <t>Organization ID</t>
   </si>
@@ -416,7 +410,7 @@
     <t>Other (explain below)</t>
   </si>
   <si>
-    <t>None</t>
+    <t>Noval</t>
   </si>
   <si>
     <t>Grant funding,Equity funding,Other (explain below)</t>
@@ -581,7 +575,25 @@
     <t>HQ Region</t>
   </si>
   <si>
-    <t>Technology</t>
+    <t>Tech 1</t>
+  </si>
+  <si>
+    <t>Tech 2</t>
+  </si>
+  <si>
+    <t>Tech 3</t>
+  </si>
+  <si>
+    <t>Tech 4</t>
+  </si>
+  <si>
+    <t>Tech 5</t>
+  </si>
+  <si>
+    <t>Tech 6</t>
+  </si>
+  <si>
+    <t>Tech 7</t>
   </si>
   <si>
     <t>Geo 1</t>
@@ -807,13 +819,25 @@
   </si>
   <si>
     <t>Manufacturing Technology</t>
+  </si>
+  <si>
+    <t>Behavioral Technology</t>
+  </si>
+  <si>
+    <t>Internet of Things</t>
+  </si>
+  <si>
+    <t>Imaging and sensor technology</t>
+  </si>
+  <si>
+    <t>Robotics and Drones</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="2" x14ac:knownFonts="1">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <fonts count="2">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -876,14 +900,6 @@
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleLight16"/>
-  <extLst>
-    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
-      <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
-    </ext>
-    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
-      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
-    </ext>
-  </extLst>
 </styleSheet>
 </file>
 
@@ -930,7 +946,7 @@
     </a:clrScheme>
     <a:fontScheme name="Office">
       <a:majorFont>
-        <a:latin typeface="Cambria" panose="020F0302020204030204"/>
+        <a:latin typeface="Cambria"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -962,27 +978,9 @@
         <a:font script="Mong" typeface="Mongolian Baiti"/>
         <a:font script="Viet" typeface="Times New Roman"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
-        <a:font script="Geor" typeface="Sylfaen"/>
-        <a:font script="Armn" typeface="Arial"/>
-        <a:font script="Bugi" typeface="Leelawadee UI"/>
-        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
-        <a:font script="Java" typeface="Javanese Text"/>
-        <a:font script="Lisu" typeface="Segoe UI"/>
-        <a:font script="Mymr" typeface="Myanmar Text"/>
-        <a:font script="Nkoo" typeface="Ebrima"/>
-        <a:font script="Olck" typeface="Nirmala UI"/>
-        <a:font script="Osma" typeface="Ebrima"/>
-        <a:font script="Phag" typeface="Phagspa"/>
-        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
-        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
-        <a:font script="Syre" typeface="Estrangelo Edessa"/>
-        <a:font script="Sora" typeface="Nirmala UI"/>
-        <a:font script="Tale" typeface="Microsoft Tai Le"/>
-        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
-        <a:font script="Tfng" typeface="Ebrima"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
+        <a:latin typeface="Calibri"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -1014,24 +1012,6 @@
         <a:font script="Mong" typeface="Mongolian Baiti"/>
         <a:font script="Viet" typeface="Arial"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
-        <a:font script="Geor" typeface="Sylfaen"/>
-        <a:font script="Armn" typeface="Arial"/>
-        <a:font script="Bugi" typeface="Leelawadee UI"/>
-        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
-        <a:font script="Java" typeface="Javanese Text"/>
-        <a:font script="Lisu" typeface="Segoe UI"/>
-        <a:font script="Mymr" typeface="Myanmar Text"/>
-        <a:font script="Nkoo" typeface="Ebrima"/>
-        <a:font script="Olck" typeface="Nirmala UI"/>
-        <a:font script="Osma" typeface="Ebrima"/>
-        <a:font script="Phag" typeface="Phagspa"/>
-        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
-        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
-        <a:font script="Syre" typeface="Estrangelo Edessa"/>
-        <a:font script="Sora" typeface="Nirmala UI"/>
-        <a:font script="Tale" typeface="Microsoft Tai Le"/>
-        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
-        <a:font script="Tfng" typeface="Ebrima"/>
       </a:minorFont>
     </a:fontScheme>
     <a:fmtScheme name="Office">
@@ -1207,22 +1187,14 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:R19"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F18" sqref="F18"/>
-    </sheetView>
+    <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
-  <cols>
-    <col min="5" max="5" width="24.59765625" customWidth="1"/>
-    <col min="6" max="6" width="53.59765625" customWidth="1"/>
-    <col min="9" max="9" width="30.53125" customWidth="1"/>
-    <col min="10" max="10" width="28.59765625" customWidth="1"/>
-  </cols>
+  <sheetFormatPr defaultRowHeight="15"/>
   <sheetData>
-    <row r="1" spans="1:18" x14ac:dyDescent="0.45">
+    <row r="1" spans="1:18">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -1278,7 +1250,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="2" spans="1:18" x14ac:dyDescent="0.45">
+    <row r="2" spans="1:18">
       <c r="A2" t="s">
         <v>18</v>
       </c>
@@ -1328,7 +1300,7 @@
         <v>177</v>
       </c>
     </row>
-    <row r="3" spans="1:18" x14ac:dyDescent="0.45">
+    <row r="3" spans="1:18">
       <c r="A3" t="s">
         <v>19</v>
       </c>
@@ -1372,7 +1344,7 @@
         <v>175</v>
       </c>
     </row>
-    <row r="4" spans="1:18" x14ac:dyDescent="0.45">
+    <row r="4" spans="1:18">
       <c r="A4" t="s">
         <v>20</v>
       </c>
@@ -1419,7 +1391,7 @@
         <v>179</v>
       </c>
     </row>
-    <row r="5" spans="1:18" x14ac:dyDescent="0.45">
+    <row r="5" spans="1:18">
       <c r="A5" t="s">
         <v>21</v>
       </c>
@@ -1460,7 +1432,7 @@
         <v>131</v>
       </c>
     </row>
-    <row r="6" spans="1:18" x14ac:dyDescent="0.45">
+    <row r="6" spans="1:18">
       <c r="A6" t="s">
         <v>22</v>
       </c>
@@ -1507,7 +1479,7 @@
         <v>174</v>
       </c>
     </row>
-    <row r="7" spans="1:18" x14ac:dyDescent="0.45">
+    <row r="7" spans="1:18">
       <c r="A7" t="s">
         <v>23</v>
       </c>
@@ -1551,7 +1523,7 @@
         <v>173</v>
       </c>
     </row>
-    <row r="8" spans="1:18" x14ac:dyDescent="0.45">
+    <row r="8" spans="1:18">
       <c r="A8" t="s">
         <v>24</v>
       </c>
@@ -1604,7 +1576,7 @@
         <v>177</v>
       </c>
     </row>
-    <row r="9" spans="1:18" x14ac:dyDescent="0.45">
+    <row r="9" spans="1:18">
       <c r="A9" t="s">
         <v>25</v>
       </c>
@@ -1648,7 +1620,7 @@
         <v>177</v>
       </c>
     </row>
-    <row r="10" spans="1:18" x14ac:dyDescent="0.45">
+    <row r="10" spans="1:18">
       <c r="A10" t="s">
         <v>26</v>
       </c>
@@ -1695,7 +1667,7 @@
         <v>173</v>
       </c>
     </row>
-    <row r="11" spans="1:18" x14ac:dyDescent="0.45">
+    <row r="11" spans="1:18">
       <c r="A11" t="s">
         <v>27</v>
       </c>
@@ -1748,7 +1720,7 @@
         <v>173</v>
       </c>
     </row>
-    <row r="12" spans="1:18" x14ac:dyDescent="0.45">
+    <row r="12" spans="1:18">
       <c r="A12" t="s">
         <v>28</v>
       </c>
@@ -1792,7 +1764,7 @@
         <v>179</v>
       </c>
     </row>
-    <row r="13" spans="1:18" x14ac:dyDescent="0.45">
+    <row r="13" spans="1:18">
       <c r="A13" t="s">
         <v>29</v>
       </c>
@@ -1836,7 +1808,7 @@
         <v>179</v>
       </c>
     </row>
-    <row r="14" spans="1:18" x14ac:dyDescent="0.45">
+    <row r="14" spans="1:18">
       <c r="A14" t="s">
         <v>30</v>
       </c>
@@ -1886,7 +1858,7 @@
         <v>179</v>
       </c>
     </row>
-    <row r="15" spans="1:18" x14ac:dyDescent="0.45">
+    <row r="15" spans="1:18">
       <c r="A15" t="s">
         <v>31</v>
       </c>
@@ -1933,7 +1905,7 @@
         <v>174</v>
       </c>
     </row>
-    <row r="16" spans="1:18" x14ac:dyDescent="0.45">
+    <row r="16" spans="1:18">
       <c r="A16" t="s">
         <v>32</v>
       </c>
@@ -1983,7 +1955,7 @@
         <v>177</v>
       </c>
     </row>
-    <row r="17" spans="1:18" x14ac:dyDescent="0.45">
+    <row r="17" spans="1:18">
       <c r="A17" t="s">
         <v>33</v>
       </c>
@@ -2033,7 +2005,7 @@
         <v>175</v>
       </c>
     </row>
-    <row r="18" spans="1:18" x14ac:dyDescent="0.45">
+    <row r="18" spans="1:18">
       <c r="A18" t="s">
         <v>34</v>
       </c>
@@ -2080,7 +2052,7 @@
         <v>173</v>
       </c>
     </row>
-    <row r="19" spans="1:18" x14ac:dyDescent="0.45">
+    <row r="19" spans="1:18">
       <c r="A19" t="s">
         <v>35</v>
       </c>
@@ -2142,17 +2114,14 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
-  <dimension ref="A1:Q44"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <dimension ref="A1:W44"/>
   <sheetViews>
-    <sheetView topLeftCell="A13" workbookViewId="0"/>
+    <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
-  <cols>
-    <col min="1" max="1" width="36.53125" customWidth="1"/>
-  </cols>
+  <sheetFormatPr defaultRowHeight="15"/>
   <sheetData>
-    <row r="1" spans="1:17" x14ac:dyDescent="0.45">
+    <row r="1" spans="1:23">
       <c r="A1" s="1" t="s">
         <v>180</v>
       </c>
@@ -2204,19 +2173,37 @@
       <c r="Q1" s="1" t="s">
         <v>189</v>
       </c>
-    </row>
-    <row r="2" spans="1:17" x14ac:dyDescent="0.45">
+      <c r="R1" s="1" t="s">
+        <v>190</v>
+      </c>
+      <c r="S1" s="1" t="s">
+        <v>191</v>
+      </c>
+      <c r="T1" s="1" t="s">
+        <v>192</v>
+      </c>
+      <c r="U1" s="1" t="s">
+        <v>193</v>
+      </c>
+      <c r="V1" s="1" t="s">
+        <v>194</v>
+      </c>
+      <c r="W1" s="1" t="s">
+        <v>195</v>
+      </c>
+    </row>
+    <row r="2" spans="1:23">
       <c r="A2" t="s">
-        <v>190</v>
+        <v>196</v>
       </c>
       <c r="B2" t="s">
-        <v>196</v>
+        <v>202</v>
       </c>
       <c r="C2" t="s">
-        <v>239</v>
+        <v>245</v>
       </c>
       <c r="D2" t="s">
-        <v>240</v>
+        <v>246</v>
       </c>
       <c r="E2" t="s">
         <v>171</v>
@@ -2237,33 +2224,51 @@
         <v>131</v>
       </c>
       <c r="K2" t="s">
-        <v>243</v>
+        <v>249</v>
       </c>
       <c r="L2" t="s">
-        <v>246</v>
+        <v>252</v>
       </c>
       <c r="M2" t="s">
-        <v>249</v>
+        <v>255</v>
       </c>
       <c r="N2" t="s">
-        <v>254</v>
+        <v>260</v>
       </c>
       <c r="O2" t="s">
-        <v>249</v>
-      </c>
-    </row>
-    <row r="3" spans="1:17" x14ac:dyDescent="0.45">
+        <v>265</v>
+      </c>
+      <c r="P2" t="s">
+        <v>269</v>
+      </c>
+      <c r="Q2" t="s">
+        <v>162</v>
+      </c>
+      <c r="R2" t="s">
+        <v>131</v>
+      </c>
+      <c r="S2" t="s">
+        <v>131</v>
+      </c>
+      <c r="T2" t="s">
+        <v>131</v>
+      </c>
+      <c r="U2" t="s">
+        <v>255</v>
+      </c>
+    </row>
+    <row r="3" spans="1:23">
       <c r="A3" t="s">
-        <v>190</v>
+        <v>196</v>
       </c>
       <c r="B3" t="s">
-        <v>197</v>
+        <v>203</v>
       </c>
       <c r="C3" t="s">
         <v>175</v>
       </c>
       <c r="D3" t="s">
-        <v>240</v>
+        <v>246</v>
       </c>
       <c r="E3" t="s">
         <v>131</v>
@@ -2284,30 +2289,48 @@
         <v>131</v>
       </c>
       <c r="K3" t="s">
-        <v>244</v>
+        <v>250</v>
       </c>
       <c r="L3" t="s">
-        <v>246</v>
+        <v>252</v>
       </c>
       <c r="M3" t="s">
-        <v>250</v>
+        <v>256</v>
       </c>
       <c r="N3" t="s">
-        <v>254</v>
+        <v>260</v>
       </c>
       <c r="O3" t="s">
-        <v>249</v>
+        <v>131</v>
       </c>
       <c r="P3" t="s">
-        <v>251</v>
-      </c>
-    </row>
-    <row r="4" spans="1:17" x14ac:dyDescent="0.45">
+        <v>131</v>
+      </c>
+      <c r="Q3" t="s">
+        <v>131</v>
+      </c>
+      <c r="R3" t="s">
+        <v>131</v>
+      </c>
+      <c r="S3" t="s">
+        <v>131</v>
+      </c>
+      <c r="T3" t="s">
+        <v>131</v>
+      </c>
+      <c r="U3" t="s">
+        <v>255</v>
+      </c>
+      <c r="V3" t="s">
+        <v>257</v>
+      </c>
+    </row>
+    <row r="4" spans="1:23">
       <c r="A4" t="s">
-        <v>190</v>
+        <v>196</v>
       </c>
       <c r="B4" t="s">
-        <v>198</v>
+        <v>204</v>
       </c>
       <c r="C4" t="s">
         <v>178</v>
@@ -2334,30 +2357,48 @@
         <v>131</v>
       </c>
       <c r="K4" t="s">
-        <v>244</v>
+        <v>250</v>
       </c>
       <c r="L4" t="s">
-        <v>247</v>
+        <v>253</v>
       </c>
       <c r="M4" t="s">
-        <v>251</v>
+        <v>257</v>
       </c>
       <c r="N4" t="s">
-        <v>255</v>
+        <v>261</v>
       </c>
       <c r="O4" t="s">
-        <v>251</v>
-      </c>
-    </row>
-    <row r="5" spans="1:17" x14ac:dyDescent="0.45">
+        <v>152</v>
+      </c>
+      <c r="P4" t="s">
+        <v>131</v>
+      </c>
+      <c r="Q4" t="s">
+        <v>131</v>
+      </c>
+      <c r="R4" t="s">
+        <v>131</v>
+      </c>
+      <c r="S4" t="s">
+        <v>131</v>
+      </c>
+      <c r="T4" t="s">
+        <v>131</v>
+      </c>
+      <c r="U4" t="s">
+        <v>257</v>
+      </c>
+    </row>
+    <row r="5" spans="1:23">
       <c r="A5" t="s">
-        <v>190</v>
+        <v>196</v>
       </c>
       <c r="B5" t="s">
-        <v>199</v>
+        <v>205</v>
       </c>
       <c r="C5" t="s">
-        <v>240</v>
+        <v>246</v>
       </c>
       <c r="D5" t="s">
         <v>171</v>
@@ -2384,30 +2425,48 @@
         <v>125</v>
       </c>
       <c r="L5" t="s">
-        <v>247</v>
+        <v>253</v>
       </c>
       <c r="M5" t="s">
-        <v>251</v>
+        <v>257</v>
       </c>
       <c r="N5" t="s">
-        <v>254</v>
+        <v>260</v>
       </c>
       <c r="O5" t="s">
-        <v>251</v>
-      </c>
-    </row>
-    <row r="6" spans="1:17" x14ac:dyDescent="0.45">
+        <v>265</v>
+      </c>
+      <c r="P5" t="s">
+        <v>264</v>
+      </c>
+      <c r="Q5" t="s">
+        <v>162</v>
+      </c>
+      <c r="R5" t="s">
+        <v>131</v>
+      </c>
+      <c r="S5" t="s">
+        <v>131</v>
+      </c>
+      <c r="T5" t="s">
+        <v>131</v>
+      </c>
+      <c r="U5" t="s">
+        <v>257</v>
+      </c>
+    </row>
+    <row r="6" spans="1:23">
       <c r="A6" t="s">
-        <v>190</v>
+        <v>196</v>
       </c>
       <c r="B6" t="s">
-        <v>200</v>
+        <v>206</v>
       </c>
       <c r="C6" t="s">
         <v>176</v>
       </c>
       <c r="D6" t="s">
-        <v>240</v>
+        <v>246</v>
       </c>
       <c r="E6" t="s">
         <v>131</v>
@@ -2431,27 +2490,45 @@
         <v>125</v>
       </c>
       <c r="L6" t="s">
-        <v>248</v>
+        <v>254</v>
       </c>
       <c r="M6" t="s">
         <v>90</v>
       </c>
       <c r="N6" t="s">
-        <v>254</v>
+        <v>260</v>
       </c>
       <c r="O6" t="s">
+        <v>262</v>
+      </c>
+      <c r="P6" t="s">
+        <v>264</v>
+      </c>
+      <c r="Q6" t="s">
+        <v>269</v>
+      </c>
+      <c r="R6" t="s">
+        <v>162</v>
+      </c>
+      <c r="S6" t="s">
+        <v>131</v>
+      </c>
+      <c r="T6" t="s">
+        <v>131</v>
+      </c>
+      <c r="U6" t="s">
         <v>90</v>
       </c>
-      <c r="P6" t="s">
-        <v>251</v>
-      </c>
-    </row>
-    <row r="7" spans="1:17" x14ac:dyDescent="0.45">
+      <c r="V6" t="s">
+        <v>257</v>
+      </c>
+    </row>
+    <row r="7" spans="1:23">
       <c r="A7" t="s">
-        <v>190</v>
+        <v>196</v>
       </c>
       <c r="B7" t="s">
-        <v>201</v>
+        <v>207</v>
       </c>
       <c r="C7" t="s">
         <v>171</v>
@@ -2460,7 +2537,7 @@
         <v>178</v>
       </c>
       <c r="E7" t="s">
-        <v>239</v>
+        <v>245</v>
       </c>
       <c r="F7" t="s">
         <v>131</v>
@@ -2481,24 +2558,42 @@
         <v>125</v>
       </c>
       <c r="L7" t="s">
-        <v>248</v>
+        <v>254</v>
       </c>
       <c r="M7" t="s">
-        <v>249</v>
+        <v>255</v>
       </c>
       <c r="N7" t="s">
         <v>162</v>
       </c>
       <c r="O7" t="s">
-        <v>249</v>
-      </c>
-    </row>
-    <row r="8" spans="1:17" x14ac:dyDescent="0.45">
+        <v>131</v>
+      </c>
+      <c r="P7" t="s">
+        <v>131</v>
+      </c>
+      <c r="Q7" t="s">
+        <v>131</v>
+      </c>
+      <c r="R7" t="s">
+        <v>131</v>
+      </c>
+      <c r="S7" t="s">
+        <v>131</v>
+      </c>
+      <c r="T7" t="s">
+        <v>131</v>
+      </c>
+      <c r="U7" t="s">
+        <v>255</v>
+      </c>
+    </row>
+    <row r="8" spans="1:23">
       <c r="A8" t="s">
-        <v>190</v>
+        <v>196</v>
       </c>
       <c r="B8" t="s">
-        <v>202</v>
+        <v>208</v>
       </c>
       <c r="C8" t="s">
         <v>171</v>
@@ -2528,27 +2623,45 @@
         <v>125</v>
       </c>
       <c r="L8" t="s">
-        <v>248</v>
+        <v>254</v>
       </c>
       <c r="M8" t="s">
         <v>95</v>
       </c>
       <c r="N8" t="s">
-        <v>256</v>
+        <v>262</v>
       </c>
       <c r="O8" t="s">
+        <v>264</v>
+      </c>
+      <c r="P8" t="s">
+        <v>162</v>
+      </c>
+      <c r="Q8" t="s">
+        <v>131</v>
+      </c>
+      <c r="R8" t="s">
+        <v>131</v>
+      </c>
+      <c r="S8" t="s">
+        <v>131</v>
+      </c>
+      <c r="T8" t="s">
+        <v>131</v>
+      </c>
+      <c r="U8" t="s">
         <v>95</v>
       </c>
     </row>
-    <row r="9" spans="1:17" x14ac:dyDescent="0.45">
+    <row r="9" spans="1:23">
       <c r="A9" t="s">
-        <v>191</v>
+        <v>197</v>
       </c>
       <c r="B9" t="s">
-        <v>203</v>
+        <v>209</v>
       </c>
       <c r="C9" t="s">
-        <v>241</v>
+        <v>247</v>
       </c>
       <c r="D9" t="s">
         <v>131</v>
@@ -2575,24 +2688,42 @@
         <v>125</v>
       </c>
       <c r="L9" t="s">
-        <v>246</v>
+        <v>252</v>
       </c>
       <c r="M9" t="s">
         <v>90</v>
       </c>
       <c r="N9" t="s">
-        <v>257</v>
+        <v>263</v>
       </c>
       <c r="O9" t="s">
+        <v>260</v>
+      </c>
+      <c r="P9" t="s">
+        <v>266</v>
+      </c>
+      <c r="Q9" t="s">
+        <v>262</v>
+      </c>
+      <c r="R9" t="s">
+        <v>264</v>
+      </c>
+      <c r="S9" t="s">
+        <v>269</v>
+      </c>
+      <c r="T9" t="s">
+        <v>162</v>
+      </c>
+      <c r="U9" t="s">
         <v>90</v>
       </c>
     </row>
-    <row r="10" spans="1:17" x14ac:dyDescent="0.45">
+    <row r="10" spans="1:23">
       <c r="A10" t="s">
-        <v>191</v>
+        <v>197</v>
       </c>
       <c r="B10" t="s">
-        <v>204</v>
+        <v>210</v>
       </c>
       <c r="C10" t="s">
         <v>176</v>
@@ -2619,30 +2750,48 @@
         <v>131</v>
       </c>
       <c r="K10" t="s">
-        <v>245</v>
+        <v>251</v>
       </c>
       <c r="L10" t="s">
-        <v>247</v>
+        <v>253</v>
       </c>
       <c r="M10" t="s">
         <v>90</v>
       </c>
       <c r="N10" t="s">
-        <v>257</v>
+        <v>263</v>
       </c>
       <c r="O10" t="s">
+        <v>264</v>
+      </c>
+      <c r="P10" t="s">
+        <v>131</v>
+      </c>
+      <c r="Q10" t="s">
+        <v>131</v>
+      </c>
+      <c r="R10" t="s">
+        <v>131</v>
+      </c>
+      <c r="S10" t="s">
+        <v>131</v>
+      </c>
+      <c r="T10" t="s">
+        <v>131</v>
+      </c>
+      <c r="U10" t="s">
         <v>90</v>
       </c>
     </row>
-    <row r="11" spans="1:17" x14ac:dyDescent="0.45">
+    <row r="11" spans="1:23">
       <c r="A11" t="s">
-        <v>191</v>
+        <v>197</v>
       </c>
       <c r="B11" t="s">
-        <v>205</v>
+        <v>211</v>
       </c>
       <c r="C11" t="s">
-        <v>239</v>
+        <v>245</v>
       </c>
       <c r="D11" t="s">
         <v>173</v>
@@ -2666,27 +2815,45 @@
         <v>131</v>
       </c>
       <c r="K11" t="s">
-        <v>245</v>
+        <v>251</v>
       </c>
       <c r="L11" t="s">
-        <v>248</v>
+        <v>254</v>
       </c>
       <c r="M11" t="s">
         <v>90</v>
       </c>
       <c r="N11" t="s">
-        <v>258</v>
+        <v>264</v>
       </c>
       <c r="O11" t="s">
+        <v>162</v>
+      </c>
+      <c r="P11" t="s">
+        <v>131</v>
+      </c>
+      <c r="Q11" t="s">
+        <v>131</v>
+      </c>
+      <c r="R11" t="s">
+        <v>131</v>
+      </c>
+      <c r="S11" t="s">
+        <v>131</v>
+      </c>
+      <c r="T11" t="s">
+        <v>131</v>
+      </c>
+      <c r="U11" t="s">
         <v>90</v>
       </c>
     </row>
-    <row r="12" spans="1:17" x14ac:dyDescent="0.45">
+    <row r="12" spans="1:23">
       <c r="A12" t="s">
-        <v>191</v>
+        <v>197</v>
       </c>
       <c r="B12" t="s">
-        <v>206</v>
+        <v>212</v>
       </c>
       <c r="C12" t="s">
         <v>173</v>
@@ -2716,24 +2883,42 @@
         <v>125</v>
       </c>
       <c r="L12" t="s">
-        <v>248</v>
+        <v>254</v>
       </c>
       <c r="M12" t="s">
         <v>90</v>
       </c>
       <c r="N12" t="s">
-        <v>257</v>
+        <v>263</v>
       </c>
       <c r="O12" t="s">
+        <v>262</v>
+      </c>
+      <c r="P12" t="s">
+        <v>131</v>
+      </c>
+      <c r="Q12" t="s">
+        <v>131</v>
+      </c>
+      <c r="R12" t="s">
+        <v>131</v>
+      </c>
+      <c r="S12" t="s">
+        <v>131</v>
+      </c>
+      <c r="T12" t="s">
+        <v>131</v>
+      </c>
+      <c r="U12" t="s">
         <v>90</v>
       </c>
     </row>
-    <row r="13" spans="1:17" x14ac:dyDescent="0.45">
+    <row r="13" spans="1:23">
       <c r="A13" t="s">
-        <v>191</v>
+        <v>197</v>
       </c>
       <c r="B13" t="s">
-        <v>207</v>
+        <v>213</v>
       </c>
       <c r="C13" t="s">
         <v>178</v>
@@ -2742,7 +2927,7 @@
         <v>176</v>
       </c>
       <c r="E13" t="s">
-        <v>241</v>
+        <v>247</v>
       </c>
       <c r="F13" t="s">
         <v>131</v>
@@ -2760,27 +2945,45 @@
         <v>131</v>
       </c>
       <c r="K13" t="s">
-        <v>245</v>
+        <v>251</v>
       </c>
       <c r="L13" t="s">
-        <v>247</v>
+        <v>253</v>
       </c>
       <c r="M13" t="s">
         <v>90</v>
       </c>
       <c r="N13" t="s">
-        <v>254</v>
+        <v>260</v>
       </c>
       <c r="O13" t="s">
+        <v>266</v>
+      </c>
+      <c r="P13" t="s">
+        <v>265</v>
+      </c>
+      <c r="Q13" t="s">
+        <v>162</v>
+      </c>
+      <c r="R13" t="s">
+        <v>131</v>
+      </c>
+      <c r="S13" t="s">
+        <v>131</v>
+      </c>
+      <c r="T13" t="s">
+        <v>131</v>
+      </c>
+      <c r="U13" t="s">
         <v>90</v>
       </c>
     </row>
-    <row r="14" spans="1:17" x14ac:dyDescent="0.45">
+    <row r="14" spans="1:23">
       <c r="A14" t="s">
-        <v>191</v>
+        <v>197</v>
       </c>
       <c r="B14" t="s">
-        <v>208</v>
+        <v>214</v>
       </c>
       <c r="C14" t="s">
         <v>175</v>
@@ -2807,27 +3010,45 @@
         <v>131</v>
       </c>
       <c r="K14" t="s">
-        <v>245</v>
+        <v>251</v>
       </c>
       <c r="L14" t="s">
-        <v>247</v>
+        <v>253</v>
       </c>
       <c r="M14" t="s">
         <v>90</v>
       </c>
       <c r="N14" t="s">
-        <v>257</v>
+        <v>263</v>
       </c>
       <c r="O14" t="s">
+        <v>264</v>
+      </c>
+      <c r="P14" t="s">
+        <v>270</v>
+      </c>
+      <c r="Q14" t="s">
+        <v>131</v>
+      </c>
+      <c r="R14" t="s">
+        <v>131</v>
+      </c>
+      <c r="S14" t="s">
+        <v>131</v>
+      </c>
+      <c r="T14" t="s">
+        <v>131</v>
+      </c>
+      <c r="U14" t="s">
         <v>90</v>
       </c>
     </row>
-    <row r="15" spans="1:17" x14ac:dyDescent="0.45">
+    <row r="15" spans="1:23">
       <c r="A15" t="s">
-        <v>191</v>
+        <v>197</v>
       </c>
       <c r="B15" t="s">
-        <v>209</v>
+        <v>215</v>
       </c>
       <c r="C15" t="s">
         <v>171</v>
@@ -2854,27 +3075,45 @@
         <v>131</v>
       </c>
       <c r="K15" t="s">
-        <v>243</v>
+        <v>249</v>
       </c>
       <c r="L15" t="s">
-        <v>247</v>
+        <v>253</v>
       </c>
       <c r="M15" t="s">
         <v>90</v>
       </c>
       <c r="N15" t="s">
-        <v>257</v>
+        <v>263</v>
       </c>
       <c r="O15" t="s">
+        <v>268</v>
+      </c>
+      <c r="P15" t="s">
+        <v>262</v>
+      </c>
+      <c r="Q15" t="s">
+        <v>162</v>
+      </c>
+      <c r="R15" t="s">
+        <v>131</v>
+      </c>
+      <c r="S15" t="s">
+        <v>131</v>
+      </c>
+      <c r="T15" t="s">
+        <v>131</v>
+      </c>
+      <c r="U15" t="s">
         <v>90</v>
       </c>
     </row>
-    <row r="16" spans="1:17" x14ac:dyDescent="0.45">
+    <row r="16" spans="1:23">
       <c r="A16" t="s">
-        <v>191</v>
+        <v>197</v>
       </c>
       <c r="B16" t="s">
-        <v>210</v>
+        <v>216</v>
       </c>
       <c r="C16" t="s">
         <v>131</v>
@@ -2901,10 +3140,10 @@
         <v>131</v>
       </c>
       <c r="K16" t="s">
-        <v>244</v>
+        <v>250</v>
       </c>
       <c r="L16" t="s">
-        <v>248</v>
+        <v>254</v>
       </c>
       <c r="M16" t="s">
         <v>90</v>
@@ -2915,19 +3154,37 @@
       <c r="O16" t="s">
         <v>131</v>
       </c>
-    </row>
-    <row r="17" spans="1:17" x14ac:dyDescent="0.45">
+      <c r="P16" t="s">
+        <v>131</v>
+      </c>
+      <c r="Q16" t="s">
+        <v>131</v>
+      </c>
+      <c r="R16" t="s">
+        <v>131</v>
+      </c>
+      <c r="S16" t="s">
+        <v>131</v>
+      </c>
+      <c r="T16" t="s">
+        <v>131</v>
+      </c>
+      <c r="U16" t="s">
+        <v>131</v>
+      </c>
+    </row>
+    <row r="17" spans="1:23">
       <c r="A17" t="s">
-        <v>192</v>
+        <v>198</v>
       </c>
       <c r="B17" t="s">
-        <v>211</v>
+        <v>217</v>
       </c>
       <c r="C17" t="s">
         <v>173</v>
       </c>
       <c r="D17" t="s">
-        <v>239</v>
+        <v>245</v>
       </c>
       <c r="E17" t="s">
         <v>131</v>
@@ -2951,33 +3208,51 @@
         <v>125</v>
       </c>
       <c r="L17" t="s">
+        <v>252</v>
+      </c>
+      <c r="M17" t="s">
+        <v>257</v>
+      </c>
+      <c r="N17" t="s">
+        <v>262</v>
+      </c>
+      <c r="O17" t="s">
+        <v>264</v>
+      </c>
+      <c r="P17" t="s">
+        <v>162</v>
+      </c>
+      <c r="Q17" t="s">
+        <v>131</v>
+      </c>
+      <c r="R17" t="s">
+        <v>131</v>
+      </c>
+      <c r="S17" t="s">
+        <v>131</v>
+      </c>
+      <c r="T17" t="s">
+        <v>131</v>
+      </c>
+      <c r="U17" t="s">
+        <v>257</v>
+      </c>
+    </row>
+    <row r="18" spans="1:23">
+      <c r="A18" t="s">
+        <v>198</v>
+      </c>
+      <c r="B18" t="s">
+        <v>218</v>
+      </c>
+      <c r="C18" t="s">
         <v>246</v>
-      </c>
-      <c r="M17" t="s">
-        <v>251</v>
-      </c>
-      <c r="N17" t="s">
-        <v>256</v>
-      </c>
-      <c r="O17" t="s">
-        <v>251</v>
-      </c>
-    </row>
-    <row r="18" spans="1:17" x14ac:dyDescent="0.45">
-      <c r="A18" t="s">
-        <v>192</v>
-      </c>
-      <c r="B18" t="s">
-        <v>212</v>
-      </c>
-      <c r="C18" t="s">
-        <v>240</v>
       </c>
       <c r="D18" t="s">
         <v>176</v>
       </c>
       <c r="E18" t="s">
-        <v>239</v>
+        <v>245</v>
       </c>
       <c r="F18" t="s">
         <v>173</v>
@@ -2995,27 +3270,45 @@
         <v>131</v>
       </c>
       <c r="K18" t="s">
-        <v>243</v>
+        <v>249</v>
       </c>
       <c r="L18" t="s">
-        <v>248</v>
+        <v>254</v>
       </c>
       <c r="M18" t="s">
-        <v>250</v>
+        <v>256</v>
       </c>
       <c r="N18" t="s">
-        <v>254</v>
+        <v>260</v>
       </c>
       <c r="O18" t="s">
-        <v>250</v>
-      </c>
-    </row>
-    <row r="19" spans="1:17" x14ac:dyDescent="0.45">
+        <v>264</v>
+      </c>
+      <c r="P18" t="s">
+        <v>270</v>
+      </c>
+      <c r="Q18" t="s">
+        <v>162</v>
+      </c>
+      <c r="R18" t="s">
+        <v>131</v>
+      </c>
+      <c r="S18" t="s">
+        <v>131</v>
+      </c>
+      <c r="T18" t="s">
+        <v>131</v>
+      </c>
+      <c r="U18" t="s">
+        <v>256</v>
+      </c>
+    </row>
+    <row r="19" spans="1:23">
       <c r="A19" t="s">
-        <v>192</v>
+        <v>198</v>
       </c>
       <c r="B19" t="s">
-        <v>213</v>
+        <v>219</v>
       </c>
       <c r="C19" t="s">
         <v>176</v>
@@ -3045,33 +3338,51 @@
         <v>125</v>
       </c>
       <c r="L19" t="s">
-        <v>248</v>
+        <v>254</v>
       </c>
       <c r="M19" t="s">
-        <v>249</v>
+        <v>255</v>
       </c>
       <c r="N19" t="s">
+        <v>265</v>
+      </c>
+      <c r="O19" t="s">
+        <v>267</v>
+      </c>
+      <c r="P19" t="s">
+        <v>131</v>
+      </c>
+      <c r="Q19" t="s">
+        <v>131</v>
+      </c>
+      <c r="R19" t="s">
+        <v>131</v>
+      </c>
+      <c r="S19" t="s">
+        <v>131</v>
+      </c>
+      <c r="T19" t="s">
+        <v>131</v>
+      </c>
+      <c r="U19" t="s">
         <v>259</v>
       </c>
-      <c r="O19" t="s">
-        <v>253</v>
-      </c>
-      <c r="P19" t="s">
-        <v>250</v>
-      </c>
-    </row>
-    <row r="20" spans="1:17" x14ac:dyDescent="0.45">
+      <c r="V19" t="s">
+        <v>256</v>
+      </c>
+    </row>
+    <row r="20" spans="1:23">
       <c r="A20" t="s">
-        <v>192</v>
+        <v>198</v>
       </c>
       <c r="B20" t="s">
-        <v>214</v>
+        <v>220</v>
       </c>
       <c r="C20" t="s">
         <v>176</v>
       </c>
       <c r="D20" t="s">
-        <v>239</v>
+        <v>245</v>
       </c>
       <c r="E20" t="s">
         <v>131</v>
@@ -3095,33 +3406,51 @@
         <v>125</v>
       </c>
       <c r="L20" t="s">
-        <v>248</v>
+        <v>254</v>
       </c>
       <c r="M20" t="s">
-        <v>251</v>
+        <v>257</v>
       </c>
       <c r="N20" t="s">
-        <v>254</v>
+        <v>260</v>
       </c>
       <c r="O20" t="s">
-        <v>251</v>
-      </c>
-    </row>
-    <row r="21" spans="1:17" x14ac:dyDescent="0.45">
+        <v>269</v>
+      </c>
+      <c r="P20" t="s">
+        <v>162</v>
+      </c>
+      <c r="Q20" t="s">
+        <v>131</v>
+      </c>
+      <c r="R20" t="s">
+        <v>131</v>
+      </c>
+      <c r="S20" t="s">
+        <v>131</v>
+      </c>
+      <c r="T20" t="s">
+        <v>131</v>
+      </c>
+      <c r="U20" t="s">
+        <v>257</v>
+      </c>
+    </row>
+    <row r="21" spans="1:23">
       <c r="A21" t="s">
-        <v>192</v>
+        <v>198</v>
       </c>
       <c r="B21" t="s">
-        <v>215</v>
+        <v>221</v>
       </c>
       <c r="C21" t="s">
-        <v>240</v>
+        <v>246</v>
       </c>
       <c r="D21" t="s">
         <v>176</v>
       </c>
       <c r="E21" t="s">
-        <v>239</v>
+        <v>245</v>
       </c>
       <c r="F21" t="s">
         <v>173</v>
@@ -3142,27 +3471,45 @@
         <v>125</v>
       </c>
       <c r="L21" t="s">
-        <v>248</v>
+        <v>254</v>
       </c>
       <c r="M21" t="s">
-        <v>252</v>
+        <v>258</v>
       </c>
       <c r="N21" t="s">
-        <v>257</v>
+        <v>263</v>
       </c>
       <c r="O21" t="s">
-        <v>252</v>
+        <v>265</v>
       </c>
       <c r="P21" t="s">
-        <v>252</v>
-      </c>
-    </row>
-    <row r="22" spans="1:17" x14ac:dyDescent="0.45">
+        <v>262</v>
+      </c>
+      <c r="Q21" t="s">
+        <v>162</v>
+      </c>
+      <c r="R21" t="s">
+        <v>131</v>
+      </c>
+      <c r="S21" t="s">
+        <v>131</v>
+      </c>
+      <c r="T21" t="s">
+        <v>131</v>
+      </c>
+      <c r="U21" t="s">
+        <v>258</v>
+      </c>
+      <c r="V21" t="s">
+        <v>258</v>
+      </c>
+    </row>
+    <row r="22" spans="1:23">
       <c r="A22" t="s">
-        <v>192</v>
+        <v>198</v>
       </c>
       <c r="B22" t="s">
-        <v>216</v>
+        <v>222</v>
       </c>
       <c r="C22" t="s">
         <v>173</v>
@@ -3171,7 +3518,7 @@
         <v>175</v>
       </c>
       <c r="E22" t="s">
-        <v>239</v>
+        <v>245</v>
       </c>
       <c r="F22" t="s">
         <v>176</v>
@@ -3189,33 +3536,51 @@
         <v>131</v>
       </c>
       <c r="K22" t="s">
-        <v>244</v>
+        <v>250</v>
       </c>
       <c r="L22" t="s">
-        <v>248</v>
+        <v>254</v>
       </c>
       <c r="M22" t="s">
-        <v>252</v>
+        <v>258</v>
       </c>
       <c r="N22" t="s">
-        <v>260</v>
+        <v>266</v>
       </c>
       <c r="O22" t="s">
-        <v>252</v>
-      </c>
-    </row>
-    <row r="23" spans="1:17" x14ac:dyDescent="0.45">
+        <v>162</v>
+      </c>
+      <c r="P22" t="s">
+        <v>131</v>
+      </c>
+      <c r="Q22" t="s">
+        <v>131</v>
+      </c>
+      <c r="R22" t="s">
+        <v>131</v>
+      </c>
+      <c r="S22" t="s">
+        <v>131</v>
+      </c>
+      <c r="T22" t="s">
+        <v>131</v>
+      </c>
+      <c r="U22" t="s">
+        <v>258</v>
+      </c>
+    </row>
+    <row r="23" spans="1:23">
       <c r="A23" t="s">
-        <v>192</v>
+        <v>198</v>
       </c>
       <c r="B23" t="s">
-        <v>217</v>
+        <v>223</v>
       </c>
       <c r="C23" t="s">
         <v>175</v>
       </c>
       <c r="D23" t="s">
-        <v>241</v>
+        <v>247</v>
       </c>
       <c r="E23" t="s">
         <v>131</v>
@@ -3236,30 +3601,48 @@
         <v>131</v>
       </c>
       <c r="K23" t="s">
-        <v>244</v>
+        <v>250</v>
       </c>
       <c r="L23" t="s">
-        <v>248</v>
+        <v>254</v>
       </c>
       <c r="M23" t="s">
         <v>90</v>
       </c>
       <c r="N23" t="s">
-        <v>260</v>
+        <v>266</v>
       </c>
       <c r="O23" t="s">
+        <v>162</v>
+      </c>
+      <c r="P23" t="s">
+        <v>131</v>
+      </c>
+      <c r="Q23" t="s">
+        <v>131</v>
+      </c>
+      <c r="R23" t="s">
+        <v>131</v>
+      </c>
+      <c r="S23" t="s">
+        <v>131</v>
+      </c>
+      <c r="T23" t="s">
+        <v>131</v>
+      </c>
+      <c r="U23" t="s">
         <v>90</v>
       </c>
     </row>
-    <row r="24" spans="1:17" x14ac:dyDescent="0.45">
+    <row r="24" spans="1:23">
       <c r="A24" t="s">
-        <v>193</v>
+        <v>199</v>
       </c>
       <c r="B24" t="s">
-        <v>218</v>
+        <v>224</v>
       </c>
       <c r="C24" t="s">
-        <v>239</v>
+        <v>245</v>
       </c>
       <c r="D24" t="s">
         <v>174</v>
@@ -3268,7 +3651,7 @@
         <v>176</v>
       </c>
       <c r="F24" t="s">
-        <v>240</v>
+        <v>246</v>
       </c>
       <c r="G24" t="s">
         <v>173</v>
@@ -3283,30 +3666,48 @@
         <v>131</v>
       </c>
       <c r="K24" t="s">
-        <v>244</v>
+        <v>250</v>
       </c>
       <c r="L24" t="s">
-        <v>246</v>
+        <v>252</v>
       </c>
       <c r="M24" t="s">
-        <v>252</v>
+        <v>258</v>
       </c>
       <c r="N24" t="s">
-        <v>260</v>
+        <v>266</v>
       </c>
       <c r="O24" t="s">
-        <v>252</v>
-      </c>
-    </row>
-    <row r="25" spans="1:17" x14ac:dyDescent="0.45">
+        <v>162</v>
+      </c>
+      <c r="P24" t="s">
+        <v>131</v>
+      </c>
+      <c r="Q24" t="s">
+        <v>131</v>
+      </c>
+      <c r="R24" t="s">
+        <v>131</v>
+      </c>
+      <c r="S24" t="s">
+        <v>131</v>
+      </c>
+      <c r="T24" t="s">
+        <v>131</v>
+      </c>
+      <c r="U24" t="s">
+        <v>258</v>
+      </c>
+    </row>
+    <row r="25" spans="1:23">
       <c r="A25" t="s">
-        <v>193</v>
+        <v>199</v>
       </c>
       <c r="B25" t="s">
-        <v>219</v>
+        <v>225</v>
       </c>
       <c r="C25" t="s">
-        <v>239</v>
+        <v>245</v>
       </c>
       <c r="D25" t="s">
         <v>175</v>
@@ -3315,7 +3716,7 @@
         <v>171</v>
       </c>
       <c r="F25" t="s">
-        <v>241</v>
+        <v>247</v>
       </c>
       <c r="G25" t="s">
         <v>174</v>
@@ -3330,39 +3731,57 @@
         <v>131</v>
       </c>
       <c r="K25" t="s">
-        <v>244</v>
+        <v>250</v>
       </c>
       <c r="L25" t="s">
-        <v>248</v>
+        <v>254</v>
       </c>
       <c r="M25" t="s">
         <v>90</v>
       </c>
       <c r="N25" t="s">
-        <v>260</v>
+        <v>266</v>
       </c>
       <c r="O25" t="s">
-        <v>251</v>
+        <v>268</v>
       </c>
       <c r="P25" t="s">
-        <v>249</v>
+        <v>265</v>
       </c>
       <c r="Q25" t="s">
+        <v>262</v>
+      </c>
+      <c r="R25" t="s">
+        <v>162</v>
+      </c>
+      <c r="S25" t="s">
+        <v>131</v>
+      </c>
+      <c r="T25" t="s">
+        <v>131</v>
+      </c>
+      <c r="U25" t="s">
+        <v>257</v>
+      </c>
+      <c r="V25" t="s">
+        <v>255</v>
+      </c>
+      <c r="W25" t="s">
         <v>90</v>
       </c>
     </row>
-    <row r="26" spans="1:17" x14ac:dyDescent="0.45">
+    <row r="26" spans="1:23">
       <c r="A26" t="s">
-        <v>193</v>
+        <v>199</v>
       </c>
       <c r="B26" t="s">
-        <v>220</v>
+        <v>226</v>
       </c>
       <c r="C26" t="s">
-        <v>240</v>
+        <v>246</v>
       </c>
       <c r="D26" t="s">
-        <v>239</v>
+        <v>245</v>
       </c>
       <c r="E26" t="s">
         <v>176</v>
@@ -3383,30 +3802,48 @@
         <v>131</v>
       </c>
       <c r="K26" t="s">
-        <v>244</v>
+        <v>250</v>
       </c>
       <c r="L26" t="s">
         <v>122</v>
       </c>
       <c r="M26" t="s">
-        <v>251</v>
+        <v>257</v>
       </c>
       <c r="N26" t="s">
-        <v>254</v>
+        <v>260</v>
       </c>
       <c r="O26" t="s">
-        <v>251</v>
-      </c>
-    </row>
-    <row r="27" spans="1:17" x14ac:dyDescent="0.45">
+        <v>162</v>
+      </c>
+      <c r="P26" t="s">
+        <v>131</v>
+      </c>
+      <c r="Q26" t="s">
+        <v>131</v>
+      </c>
+      <c r="R26" t="s">
+        <v>131</v>
+      </c>
+      <c r="S26" t="s">
+        <v>131</v>
+      </c>
+      <c r="T26" t="s">
+        <v>131</v>
+      </c>
+      <c r="U26" t="s">
+        <v>257</v>
+      </c>
+    </row>
+    <row r="27" spans="1:23">
       <c r="A27" t="s">
-        <v>193</v>
+        <v>199</v>
       </c>
       <c r="B27" t="s">
-        <v>221</v>
+        <v>227</v>
       </c>
       <c r="C27" t="s">
-        <v>241</v>
+        <v>247</v>
       </c>
       <c r="D27" t="s">
         <v>131</v>
@@ -3433,33 +3870,51 @@
         <v>125</v>
       </c>
       <c r="L27" t="s">
-        <v>246</v>
+        <v>252</v>
       </c>
       <c r="M27" t="s">
-        <v>249</v>
+        <v>255</v>
       </c>
       <c r="N27" t="s">
-        <v>259</v>
+        <v>265</v>
       </c>
       <c r="O27" t="s">
-        <v>249</v>
-      </c>
-    </row>
-    <row r="28" spans="1:17" x14ac:dyDescent="0.45">
+        <v>262</v>
+      </c>
+      <c r="P27" t="s">
+        <v>162</v>
+      </c>
+      <c r="Q27" t="s">
+        <v>131</v>
+      </c>
+      <c r="R27" t="s">
+        <v>131</v>
+      </c>
+      <c r="S27" t="s">
+        <v>131</v>
+      </c>
+      <c r="T27" t="s">
+        <v>131</v>
+      </c>
+      <c r="U27" t="s">
+        <v>255</v>
+      </c>
+    </row>
+    <row r="28" spans="1:23">
       <c r="A28" t="s">
-        <v>193</v>
+        <v>199</v>
       </c>
       <c r="B28" t="s">
-        <v>222</v>
+        <v>228</v>
       </c>
       <c r="C28" t="s">
         <v>176</v>
       </c>
       <c r="D28" t="s">
-        <v>240</v>
+        <v>246</v>
       </c>
       <c r="E28" t="s">
-        <v>239</v>
+        <v>245</v>
       </c>
       <c r="F28" t="s">
         <v>131</v>
@@ -3477,33 +3932,51 @@
         <v>131</v>
       </c>
       <c r="K28" t="s">
-        <v>243</v>
+        <v>249</v>
       </c>
       <c r="L28" t="s">
-        <v>246</v>
+        <v>252</v>
       </c>
       <c r="M28" t="s">
         <v>95</v>
       </c>
       <c r="N28" t="s">
-        <v>260</v>
+        <v>266</v>
       </c>
       <c r="O28" t="s">
+        <v>131</v>
+      </c>
+      <c r="P28" t="s">
+        <v>131</v>
+      </c>
+      <c r="Q28" t="s">
+        <v>131</v>
+      </c>
+      <c r="R28" t="s">
+        <v>131</v>
+      </c>
+      <c r="S28" t="s">
+        <v>131</v>
+      </c>
+      <c r="T28" t="s">
+        <v>131</v>
+      </c>
+      <c r="U28" t="s">
         <v>95</v>
       </c>
     </row>
-    <row r="29" spans="1:17" x14ac:dyDescent="0.45">
+    <row r="29" spans="1:23">
       <c r="A29" t="s">
-        <v>193</v>
+        <v>199</v>
       </c>
       <c r="B29" t="s">
-        <v>223</v>
+        <v>229</v>
       </c>
       <c r="C29" t="s">
         <v>175</v>
       </c>
       <c r="D29" t="s">
-        <v>241</v>
+        <v>247</v>
       </c>
       <c r="E29" t="s">
         <v>171</v>
@@ -3512,7 +3985,7 @@
         <v>174</v>
       </c>
       <c r="G29" t="s">
-        <v>239</v>
+        <v>245</v>
       </c>
       <c r="H29" t="s">
         <v>173</v>
@@ -3524,45 +3997,63 @@
         <v>131</v>
       </c>
       <c r="K29" t="s">
-        <v>244</v>
+        <v>250</v>
       </c>
       <c r="L29" t="s">
-        <v>248</v>
+        <v>254</v>
       </c>
       <c r="M29" t="s">
-        <v>250</v>
+        <v>256</v>
       </c>
       <c r="N29" t="s">
-        <v>260</v>
+        <v>266</v>
       </c>
       <c r="O29" t="s">
-        <v>253</v>
+        <v>162</v>
       </c>
       <c r="P29" t="s">
-        <v>253</v>
-      </c>
-    </row>
-    <row r="30" spans="1:17" x14ac:dyDescent="0.45">
+        <v>131</v>
+      </c>
+      <c r="Q29" t="s">
+        <v>131</v>
+      </c>
+      <c r="R29" t="s">
+        <v>131</v>
+      </c>
+      <c r="S29" t="s">
+        <v>131</v>
+      </c>
+      <c r="T29" t="s">
+        <v>131</v>
+      </c>
+      <c r="U29" t="s">
+        <v>259</v>
+      </c>
+      <c r="V29" t="s">
+        <v>259</v>
+      </c>
+    </row>
+    <row r="30" spans="1:23">
       <c r="A30" t="s">
-        <v>193</v>
+        <v>199</v>
       </c>
       <c r="B30" t="s">
-        <v>224</v>
+        <v>230</v>
       </c>
       <c r="C30" t="s">
         <v>171</v>
       </c>
       <c r="D30" t="s">
-        <v>242</v>
+        <v>248</v>
       </c>
       <c r="E30" t="s">
         <v>176</v>
       </c>
       <c r="F30" t="s">
-        <v>241</v>
+        <v>247</v>
       </c>
       <c r="G30" t="s">
-        <v>239</v>
+        <v>245</v>
       </c>
       <c r="H30" t="s">
         <v>131</v>
@@ -3574,27 +4065,45 @@
         <v>131</v>
       </c>
       <c r="K30" t="s">
-        <v>244</v>
+        <v>250</v>
       </c>
       <c r="L30" t="s">
-        <v>246</v>
+        <v>252</v>
       </c>
       <c r="M30" t="s">
-        <v>249</v>
+        <v>255</v>
       </c>
       <c r="N30" t="s">
-        <v>259</v>
+        <v>265</v>
       </c>
       <c r="O30" t="s">
-        <v>249</v>
-      </c>
-    </row>
-    <row r="31" spans="1:17" x14ac:dyDescent="0.45">
+        <v>162</v>
+      </c>
+      <c r="P30" t="s">
+        <v>131</v>
+      </c>
+      <c r="Q30" t="s">
+        <v>131</v>
+      </c>
+      <c r="R30" t="s">
+        <v>131</v>
+      </c>
+      <c r="S30" t="s">
+        <v>131</v>
+      </c>
+      <c r="T30" t="s">
+        <v>131</v>
+      </c>
+      <c r="U30" t="s">
+        <v>255</v>
+      </c>
+    </row>
+    <row r="31" spans="1:23">
       <c r="A31" t="s">
-        <v>194</v>
+        <v>200</v>
       </c>
       <c r="B31" t="s">
-        <v>225</v>
+        <v>231</v>
       </c>
       <c r="C31" t="s">
         <v>178</v>
@@ -3621,30 +4130,48 @@
         <v>131</v>
       </c>
       <c r="K31" t="s">
-        <v>243</v>
+        <v>249</v>
       </c>
       <c r="L31" t="s">
-        <v>247</v>
+        <v>253</v>
       </c>
       <c r="M31" t="s">
-        <v>251</v>
+        <v>257</v>
       </c>
       <c r="N31" t="s">
-        <v>261</v>
+        <v>267</v>
       </c>
       <c r="O31" t="s">
-        <v>251</v>
-      </c>
-    </row>
-    <row r="32" spans="1:17" x14ac:dyDescent="0.45">
+        <v>131</v>
+      </c>
+      <c r="P31" t="s">
+        <v>131</v>
+      </c>
+      <c r="Q31" t="s">
+        <v>131</v>
+      </c>
+      <c r="R31" t="s">
+        <v>131</v>
+      </c>
+      <c r="S31" t="s">
+        <v>131</v>
+      </c>
+      <c r="T31" t="s">
+        <v>131</v>
+      </c>
+      <c r="U31" t="s">
+        <v>257</v>
+      </c>
+    </row>
+    <row r="32" spans="1:23">
       <c r="A32" t="s">
-        <v>194</v>
+        <v>200</v>
       </c>
       <c r="B32" t="s">
-        <v>226</v>
+        <v>232</v>
       </c>
       <c r="C32" t="s">
-        <v>240</v>
+        <v>246</v>
       </c>
       <c r="D32" t="s">
         <v>131</v>
@@ -3671,24 +4198,42 @@
         <v>125</v>
       </c>
       <c r="L32" t="s">
-        <v>248</v>
+        <v>254</v>
       </c>
       <c r="M32" t="s">
-        <v>249</v>
+        <v>255</v>
       </c>
       <c r="N32" t="s">
-        <v>260</v>
+        <v>266</v>
       </c>
       <c r="O32" t="s">
-        <v>249</v>
-      </c>
-    </row>
-    <row r="33" spans="1:16" x14ac:dyDescent="0.45">
+        <v>270</v>
+      </c>
+      <c r="P32" t="s">
+        <v>162</v>
+      </c>
+      <c r="Q32" t="s">
+        <v>131</v>
+      </c>
+      <c r="R32" t="s">
+        <v>131</v>
+      </c>
+      <c r="S32" t="s">
+        <v>131</v>
+      </c>
+      <c r="T32" t="s">
+        <v>131</v>
+      </c>
+      <c r="U32" t="s">
+        <v>255</v>
+      </c>
+    </row>
+    <row r="33" spans="1:22">
       <c r="A33" t="s">
-        <v>194</v>
+        <v>200</v>
       </c>
       <c r="B33" t="s">
-        <v>227</v>
+        <v>233</v>
       </c>
       <c r="C33" t="s">
         <v>178</v>
@@ -3700,7 +4245,7 @@
         <v>172</v>
       </c>
       <c r="F33" t="s">
-        <v>240</v>
+        <v>246</v>
       </c>
       <c r="G33" t="s">
         <v>131</v>
@@ -3718,24 +4263,42 @@
         <v>125</v>
       </c>
       <c r="L33" t="s">
-        <v>248</v>
+        <v>254</v>
       </c>
       <c r="M33" t="s">
-        <v>249</v>
+        <v>255</v>
       </c>
       <c r="N33" t="s">
-        <v>257</v>
+        <v>263</v>
       </c>
       <c r="O33" t="s">
-        <v>249</v>
-      </c>
-    </row>
-    <row r="34" spans="1:16" x14ac:dyDescent="0.45">
+        <v>260</v>
+      </c>
+      <c r="P33" t="s">
+        <v>268</v>
+      </c>
+      <c r="Q33" t="s">
+        <v>265</v>
+      </c>
+      <c r="R33" t="s">
+        <v>262</v>
+      </c>
+      <c r="S33" t="s">
+        <v>162</v>
+      </c>
+      <c r="T33" t="s">
+        <v>131</v>
+      </c>
+      <c r="U33" t="s">
+        <v>255</v>
+      </c>
+    </row>
+    <row r="34" spans="1:22">
       <c r="A34" t="s">
-        <v>194</v>
+        <v>200</v>
       </c>
       <c r="B34" t="s">
-        <v>228</v>
+        <v>234</v>
       </c>
       <c r="C34" t="s">
         <v>171</v>
@@ -3762,27 +4325,45 @@
         <v>131</v>
       </c>
       <c r="K34" t="s">
-        <v>243</v>
+        <v>249</v>
       </c>
       <c r="L34" t="s">
-        <v>247</v>
+        <v>253</v>
       </c>
       <c r="M34" t="s">
         <v>90</v>
       </c>
       <c r="N34" t="s">
-        <v>261</v>
+        <v>267</v>
       </c>
       <c r="O34" t="s">
-        <v>249</v>
-      </c>
-    </row>
-    <row r="35" spans="1:16" x14ac:dyDescent="0.45">
+        <v>131</v>
+      </c>
+      <c r="P34" t="s">
+        <v>131</v>
+      </c>
+      <c r="Q34" t="s">
+        <v>131</v>
+      </c>
+      <c r="R34" t="s">
+        <v>131</v>
+      </c>
+      <c r="S34" t="s">
+        <v>131</v>
+      </c>
+      <c r="T34" t="s">
+        <v>131</v>
+      </c>
+      <c r="U34" t="s">
+        <v>255</v>
+      </c>
+    </row>
+    <row r="35" spans="1:22">
       <c r="A35" t="s">
-        <v>194</v>
+        <v>200</v>
       </c>
       <c r="B35" t="s">
-        <v>229</v>
+        <v>235</v>
       </c>
       <c r="C35" t="s">
         <v>178</v>
@@ -3791,16 +4372,16 @@
         <v>176</v>
       </c>
       <c r="E35" t="s">
-        <v>241</v>
+        <v>247</v>
       </c>
       <c r="F35" t="s">
         <v>171</v>
       </c>
       <c r="G35" t="s">
-        <v>239</v>
+        <v>245</v>
       </c>
       <c r="H35" t="s">
-        <v>240</v>
+        <v>246</v>
       </c>
       <c r="I35" t="s">
         <v>131</v>
@@ -3809,27 +4390,45 @@
         <v>131</v>
       </c>
       <c r="K35" t="s">
-        <v>243</v>
+        <v>249</v>
       </c>
       <c r="L35" t="s">
-        <v>248</v>
+        <v>254</v>
       </c>
       <c r="M35" t="s">
-        <v>251</v>
+        <v>257</v>
       </c>
       <c r="N35" t="s">
-        <v>254</v>
+        <v>260</v>
       </c>
       <c r="O35" t="s">
-        <v>251</v>
-      </c>
-    </row>
-    <row r="36" spans="1:16" x14ac:dyDescent="0.45">
+        <v>268</v>
+      </c>
+      <c r="P35" t="s">
+        <v>265</v>
+      </c>
+      <c r="Q35" t="s">
+        <v>269</v>
+      </c>
+      <c r="R35" t="s">
+        <v>162</v>
+      </c>
+      <c r="S35" t="s">
+        <v>131</v>
+      </c>
+      <c r="T35" t="s">
+        <v>131</v>
+      </c>
+      <c r="U35" t="s">
+        <v>257</v>
+      </c>
+    </row>
+    <row r="36" spans="1:22">
       <c r="A36" t="s">
-        <v>194</v>
+        <v>200</v>
       </c>
       <c r="B36" t="s">
-        <v>230</v>
+        <v>236</v>
       </c>
       <c r="C36" t="s">
         <v>173</v>
@@ -3859,24 +4458,42 @@
         <v>125</v>
       </c>
       <c r="L36" t="s">
-        <v>247</v>
+        <v>253</v>
       </c>
       <c r="M36" t="s">
         <v>90</v>
       </c>
       <c r="N36" t="s">
-        <v>254</v>
+        <v>260</v>
       </c>
       <c r="O36" t="s">
+        <v>162</v>
+      </c>
+      <c r="P36" t="s">
+        <v>131</v>
+      </c>
+      <c r="Q36" t="s">
+        <v>131</v>
+      </c>
+      <c r="R36" t="s">
+        <v>131</v>
+      </c>
+      <c r="S36" t="s">
+        <v>131</v>
+      </c>
+      <c r="T36" t="s">
+        <v>131</v>
+      </c>
+      <c r="U36" t="s">
         <v>90</v>
       </c>
     </row>
-    <row r="37" spans="1:16" x14ac:dyDescent="0.45">
+    <row r="37" spans="1:22">
       <c r="A37" t="s">
-        <v>194</v>
+        <v>200</v>
       </c>
       <c r="B37" t="s">
-        <v>231</v>
+        <v>237</v>
       </c>
       <c r="C37" t="s">
         <v>171</v>
@@ -3894,36 +4511,54 @@
         <v>176</v>
       </c>
       <c r="H37" t="s">
-        <v>241</v>
+        <v>247</v>
       </c>
       <c r="I37" t="s">
-        <v>239</v>
+        <v>245</v>
       </c>
       <c r="J37" t="s">
-        <v>240</v>
+        <v>246</v>
       </c>
       <c r="K37" t="s">
-        <v>243</v>
+        <v>249</v>
       </c>
       <c r="L37" t="s">
-        <v>247</v>
+        <v>253</v>
       </c>
       <c r="M37" t="s">
         <v>90</v>
       </c>
       <c r="N37" t="s">
-        <v>255</v>
+        <v>261</v>
       </c>
       <c r="O37" t="s">
+        <v>131</v>
+      </c>
+      <c r="P37" t="s">
+        <v>131</v>
+      </c>
+      <c r="Q37" t="s">
+        <v>131</v>
+      </c>
+      <c r="R37" t="s">
+        <v>131</v>
+      </c>
+      <c r="S37" t="s">
+        <v>131</v>
+      </c>
+      <c r="T37" t="s">
+        <v>131</v>
+      </c>
+      <c r="U37" t="s">
         <v>90</v>
       </c>
     </row>
-    <row r="38" spans="1:16" x14ac:dyDescent="0.45">
+    <row r="38" spans="1:22">
       <c r="A38" t="s">
-        <v>195</v>
+        <v>201</v>
       </c>
       <c r="B38" t="s">
-        <v>232</v>
+        <v>238</v>
       </c>
       <c r="C38" t="s">
         <v>173</v>
@@ -3953,27 +4588,45 @@
         <v>125</v>
       </c>
       <c r="L38" t="s">
-        <v>246</v>
+        <v>252</v>
       </c>
       <c r="M38" t="s">
         <v>95</v>
       </c>
       <c r="N38" t="s">
+        <v>261</v>
+      </c>
+      <c r="O38" t="s">
+        <v>131</v>
+      </c>
+      <c r="P38" t="s">
+        <v>131</v>
+      </c>
+      <c r="Q38" t="s">
+        <v>131</v>
+      </c>
+      <c r="R38" t="s">
+        <v>131</v>
+      </c>
+      <c r="S38" t="s">
+        <v>131</v>
+      </c>
+      <c r="T38" t="s">
+        <v>131</v>
+      </c>
+      <c r="U38" t="s">
+        <v>95</v>
+      </c>
+      <c r="V38" t="s">
         <v>255</v>
       </c>
-      <c r="O38" t="s">
-        <v>95</v>
-      </c>
-      <c r="P38" t="s">
-        <v>249</v>
-      </c>
-    </row>
-    <row r="39" spans="1:16" x14ac:dyDescent="0.45">
+    </row>
+    <row r="39" spans="1:22">
       <c r="A39" t="s">
-        <v>195</v>
+        <v>201</v>
       </c>
       <c r="B39" t="s">
-        <v>233</v>
+        <v>239</v>
       </c>
       <c r="C39" t="s">
         <v>173</v>
@@ -4003,33 +4656,51 @@
         <v>125</v>
       </c>
       <c r="L39" t="s">
-        <v>246</v>
+        <v>252</v>
       </c>
       <c r="M39" t="s">
-        <v>253</v>
+        <v>259</v>
       </c>
       <c r="N39" t="s">
-        <v>254</v>
+        <v>260</v>
       </c>
       <c r="O39" t="s">
+        <v>265</v>
+      </c>
+      <c r="P39" t="s">
+        <v>270</v>
+      </c>
+      <c r="Q39" t="s">
+        <v>269</v>
+      </c>
+      <c r="R39" t="s">
+        <v>271</v>
+      </c>
+      <c r="S39" t="s">
+        <v>162</v>
+      </c>
+      <c r="T39" t="s">
+        <v>131</v>
+      </c>
+      <c r="U39" t="s">
         <v>90</v>
       </c>
-      <c r="P39" t="s">
-        <v>253</v>
-      </c>
-    </row>
-    <row r="40" spans="1:16" x14ac:dyDescent="0.45">
+      <c r="V39" t="s">
+        <v>259</v>
+      </c>
+    </row>
+    <row r="40" spans="1:22">
       <c r="A40" t="s">
-        <v>195</v>
+        <v>201</v>
       </c>
       <c r="B40" t="s">
-        <v>234</v>
+        <v>240</v>
       </c>
       <c r="C40" t="s">
         <v>176</v>
       </c>
       <c r="D40" t="s">
-        <v>239</v>
+        <v>245</v>
       </c>
       <c r="E40" t="s">
         <v>131</v>
@@ -4053,27 +4724,45 @@
         <v>125</v>
       </c>
       <c r="L40" t="s">
+        <v>253</v>
+      </c>
+      <c r="M40" t="s">
+        <v>259</v>
+      </c>
+      <c r="N40" t="s">
+        <v>261</v>
+      </c>
+      <c r="O40" t="s">
+        <v>270</v>
+      </c>
+      <c r="P40" t="s">
+        <v>269</v>
+      </c>
+      <c r="Q40" t="s">
+        <v>271</v>
+      </c>
+      <c r="R40" t="s">
+        <v>131</v>
+      </c>
+      <c r="S40" t="s">
+        <v>131</v>
+      </c>
+      <c r="T40" t="s">
+        <v>131</v>
+      </c>
+      <c r="U40" t="s">
+        <v>259</v>
+      </c>
+    </row>
+    <row r="41" spans="1:22">
+      <c r="A41" t="s">
+        <v>201</v>
+      </c>
+      <c r="B41" t="s">
+        <v>241</v>
+      </c>
+      <c r="C41" t="s">
         <v>247</v>
-      </c>
-      <c r="M40" t="s">
-        <v>253</v>
-      </c>
-      <c r="N40" t="s">
-        <v>255</v>
-      </c>
-      <c r="O40" t="s">
-        <v>253</v>
-      </c>
-    </row>
-    <row r="41" spans="1:16" x14ac:dyDescent="0.45">
-      <c r="A41" t="s">
-        <v>195</v>
-      </c>
-      <c r="B41" t="s">
-        <v>235</v>
-      </c>
-      <c r="C41" t="s">
-        <v>241</v>
       </c>
       <c r="D41" t="s">
         <v>131</v>
@@ -4100,77 +4789,113 @@
         <v>125</v>
       </c>
       <c r="L41" t="s">
-        <v>248</v>
+        <v>254</v>
       </c>
       <c r="M41" t="s">
+        <v>255</v>
+      </c>
+      <c r="N41" t="s">
+        <v>267</v>
+      </c>
+      <c r="O41" t="s">
+        <v>131</v>
+      </c>
+      <c r="P41" t="s">
+        <v>131</v>
+      </c>
+      <c r="Q41" t="s">
+        <v>131</v>
+      </c>
+      <c r="R41" t="s">
+        <v>131</v>
+      </c>
+      <c r="S41" t="s">
+        <v>131</v>
+      </c>
+      <c r="T41" t="s">
+        <v>131</v>
+      </c>
+      <c r="U41" t="s">
+        <v>255</v>
+      </c>
+    </row>
+    <row r="42" spans="1:22">
+      <c r="A42" t="s">
+        <v>201</v>
+      </c>
+      <c r="B42" t="s">
+        <v>242</v>
+      </c>
+      <c r="C42" t="s">
+        <v>247</v>
+      </c>
+      <c r="D42" t="s">
+        <v>131</v>
+      </c>
+      <c r="E42" t="s">
+        <v>131</v>
+      </c>
+      <c r="F42" t="s">
+        <v>131</v>
+      </c>
+      <c r="G42" t="s">
+        <v>131</v>
+      </c>
+      <c r="H42" t="s">
+        <v>131</v>
+      </c>
+      <c r="I42" t="s">
+        <v>131</v>
+      </c>
+      <c r="J42" t="s">
+        <v>131</v>
+      </c>
+      <c r="K42" t="s">
         <v>249</v>
       </c>
-      <c r="N41" t="s">
-        <v>261</v>
-      </c>
-      <c r="O41" t="s">
-        <v>249</v>
-      </c>
-    </row>
-    <row r="42" spans="1:16" x14ac:dyDescent="0.45">
-      <c r="A42" t="s">
-        <v>195</v>
-      </c>
-      <c r="B42" t="s">
-        <v>236</v>
-      </c>
-      <c r="C42" t="s">
-        <v>241</v>
-      </c>
-      <c r="D42" t="s">
-        <v>131</v>
-      </c>
-      <c r="E42" t="s">
-        <v>131</v>
-      </c>
-      <c r="F42" t="s">
-        <v>131</v>
-      </c>
-      <c r="G42" t="s">
-        <v>131</v>
-      </c>
-      <c r="H42" t="s">
-        <v>131</v>
-      </c>
-      <c r="I42" t="s">
-        <v>131</v>
-      </c>
-      <c r="J42" t="s">
-        <v>131</v>
-      </c>
-      <c r="K42" t="s">
+      <c r="L42" t="s">
+        <v>254</v>
+      </c>
+      <c r="M42" t="s">
+        <v>258</v>
+      </c>
+      <c r="N42" t="s">
+        <v>262</v>
+      </c>
+      <c r="O42" t="s">
+        <v>267</v>
+      </c>
+      <c r="P42" t="s">
+        <v>162</v>
+      </c>
+      <c r="Q42" t="s">
+        <v>131</v>
+      </c>
+      <c r="R42" t="s">
+        <v>131</v>
+      </c>
+      <c r="S42" t="s">
+        <v>131</v>
+      </c>
+      <c r="T42" t="s">
+        <v>131</v>
+      </c>
+      <c r="U42" t="s">
+        <v>258</v>
+      </c>
+    </row>
+    <row r="43" spans="1:22">
+      <c r="A43" t="s">
+        <v>201</v>
+      </c>
+      <c r="B43" t="s">
         <v>243</v>
-      </c>
-      <c r="L42" t="s">
-        <v>248</v>
-      </c>
-      <c r="M42" t="s">
-        <v>252</v>
-      </c>
-      <c r="N42" t="s">
-        <v>256</v>
-      </c>
-      <c r="O42" t="s">
-        <v>252</v>
-      </c>
-    </row>
-    <row r="43" spans="1:16" x14ac:dyDescent="0.45">
-      <c r="A43" t="s">
-        <v>195</v>
-      </c>
-      <c r="B43" t="s">
-        <v>237</v>
       </c>
       <c r="C43" t="s">
         <v>171</v>
       </c>
       <c r="D43" t="s">
-        <v>239</v>
+        <v>245</v>
       </c>
       <c r="E43" t="s">
         <v>131</v>
@@ -4194,30 +4919,48 @@
         <v>125</v>
       </c>
       <c r="L43" t="s">
-        <v>246</v>
+        <v>252</v>
       </c>
       <c r="M43" t="s">
         <v>90</v>
       </c>
       <c r="N43" t="s">
-        <v>255</v>
+        <v>261</v>
       </c>
       <c r="O43" t="s">
+        <v>152</v>
+      </c>
+      <c r="P43" t="s">
+        <v>131</v>
+      </c>
+      <c r="Q43" t="s">
+        <v>131</v>
+      </c>
+      <c r="R43" t="s">
+        <v>131</v>
+      </c>
+      <c r="S43" t="s">
+        <v>131</v>
+      </c>
+      <c r="T43" t="s">
+        <v>131</v>
+      </c>
+      <c r="U43" t="s">
         <v>90</v>
       </c>
     </row>
-    <row r="44" spans="1:16" x14ac:dyDescent="0.45">
+    <row r="44" spans="1:22">
       <c r="A44" t="s">
-        <v>195</v>
+        <v>201</v>
       </c>
       <c r="B44" t="s">
-        <v>238</v>
+        <v>244</v>
       </c>
       <c r="C44" t="s">
         <v>178</v>
       </c>
       <c r="D44" t="s">
-        <v>239</v>
+        <v>245</v>
       </c>
       <c r="E44" t="s">
         <v>131</v>
@@ -4241,16 +4984,34 @@
         <v>125</v>
       </c>
       <c r="L44" t="s">
-        <v>248</v>
+        <v>254</v>
       </c>
       <c r="M44" t="s">
-        <v>250</v>
+        <v>256</v>
       </c>
       <c r="N44" t="s">
-        <v>254</v>
+        <v>260</v>
       </c>
       <c r="O44" t="s">
-        <v>250</v>
+        <v>265</v>
+      </c>
+      <c r="P44" t="s">
+        <v>269</v>
+      </c>
+      <c r="Q44" t="s">
+        <v>162</v>
+      </c>
+      <c r="R44" t="s">
+        <v>131</v>
+      </c>
+      <c r="S44" t="s">
+        <v>131</v>
+      </c>
+      <c r="T44" t="s">
+        <v>131</v>
+      </c>
+      <c r="U44" t="s">
+        <v>256</v>
       </c>
     </row>
   </sheetData>

</xml_diff>